<commit_message>
:up: commit antes de formatar
</commit_message>
<xml_diff>
--- a/banco_de_dados/vocabulario.xlsx
+++ b/banco_de_dados/vocabulario.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,6 +1583,126 @@
         <v>0</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>infringement</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>violação</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>inextricable</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>adjective</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>inextricável</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>outrage</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>ultraje</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>vitriol</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>noun</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>vitríolo</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>towards</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>preposition</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>em relação</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>refrain</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>verb</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>abster</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>